<commit_message>
Ternary operator within parentheses for parseDate method
</commit_message>
<xml_diff>
--- a/src/main/resources/static/files_for_testing_exceptions/NullHeader.xlsx
+++ b/src/main/resources/static/files_for_testing_exceptions/NullHeader.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29113"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD829485-9834-4DF1-8E71-E1A4C99F6F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C0ADA96-3387-487E-B847-187C961B7C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Gigi</t>
+  </si>
+  <si>
+    <t>2000-07-02</t>
   </si>
   <si>
     <t>MALE</t>
@@ -90,9 +93,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -431,29 +435,32 @@
   <dimension ref="A2:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>45</v>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>

</xml_diff>